<commit_message>
Change Most Common Words Top 20 to 10
</commit_message>
<xml_diff>
--- a/songs_ranking.xlsx
+++ b/songs_ranking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\论文\预答辩\lyrics_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC20A2A-BEC1-462F-A789-120D18C55291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8B2EFD-0B20-4777-AE28-FEA97936F643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{093EF821-A1CC-49CE-B51C-78C85399FFF4}"/>
+    <workbookView xWindow="14115" yWindow="3615" windowWidth="14475" windowHeight="11332" xr2:uid="{093EF821-A1CC-49CE-B51C-78C85399FFF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -687,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92620CE8-8840-4994-829B-9D8808D3D62A}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="38.59765625" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -895,7 +895,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="4">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">

</xml_diff>